<commit_message>
Aggiunti nuovi commenti e analisi su Claude Sonnet
</commit_message>
<xml_diff>
--- a/HE/W_in_progress/Ulteriori_analisi/Residui_human_eval_metriche.xlsx
+++ b/HE/W_in_progress/Ulteriori_analisi/Residui_human_eval_metriche.xlsx
@@ -8,17 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcd\Desktop\Tesi\Work\repo\Tesi_Generatore_VHDL\HE\W_in_progress\Ulteriori_analisi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8856F9FD-3C60-4648-A42B-65FC2D9CBFEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985F04ED-C514-457E-8CF8-254D6A999332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="23280" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36150" yWindow="0" windowWidth="17250" windowHeight="8865" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Residui" sheetId="1" r:id="rId1"/>
+    <sheet name="Foglio1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Tabelle1!$D$2:$D$5</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Tabelle1!$D$2:$D$5</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
   <si>
     <t>CodeGen</t>
   </si>
@@ -107,10 +104,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -156,7 +154,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -174,17 +172,7 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="9.3136701662292209E-2"/>
-          <c:y val="0.19721055701370663"/>
-          <c:w val="0.87630774278215218"/>
-          <c:h val="0.77736111111111106"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -192,9 +180,20 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Residuals</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent2"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -202,9 +201,66 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$A$2:$A$6</c:f>
+              <c:f>Foglio1!$B$3:$B$7</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -227,7 +283,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$D$2:$D$6</c:f>
+              <c:f>Foglio1!$E$3:$E$7</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -244,37 +300,52 @@
                   <c:v>-0.12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>-0.69</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9B59-4164-8553-052AE791B71A}"/>
+              <c16:uniqueId val="{00000000-4C1E-4AC8-97E3-C5766F36132E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="610742095"/>
-        <c:axId val="610742575"/>
+        <c:gapWidth val="444"/>
+        <c:overlap val="-90"/>
+        <c:axId val="554565440"/>
+        <c:axId val="554575520"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="610742095"/>
+        <c:axId val="554565440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -297,7 +368,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -312,7 +383,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="610742575"/>
+        <c:crossAx val="554575520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -320,58 +391,17 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="610742575"/>
+        <c:axId val="554575520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="610742095"/>
+        <c:crossAx val="554565440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -396,7 +426,7 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="lt1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
@@ -468,7 +498,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="202">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -479,7 +509,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -502,18 +532,18 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="bg1"/>
+        <a:schemeClr val="lt1"/>
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
@@ -525,7 +555,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -533,11 +563,14 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -569,35 +602,45 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -609,30 +652,34 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -654,15 +701,13 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -677,10 +722,46 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
@@ -688,67 +769,128 @@
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -761,54 +903,17 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -818,8 +923,8 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
+  </cs:seriesLine>
+  <cs:title>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -829,66 +934,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -897,14 +943,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -918,7 +964,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="800" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
@@ -934,8 +980,8 @@
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -951,6 +997,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -958,14 +1015,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -974,23 +1025,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>662940</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>148590</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>16192</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1165860</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>148590</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>40957</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Grafico 4">
+        <xdr:cNvPr id="4" name="Grafico 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCFE8A03-5C4E-1063-4E84-D27D2723D340}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A416F6B-C92D-E30C-7F39-ABB42EE4A764}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1276,8 +1327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1376,6 +1427,109 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCF6B64A-97C8-4962-87E8-262A3ABBAE56}">
+  <dimension ref="B2:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="23.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.76</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" ref="E3" si="0">SUM(-C3,D3)</f>
+        <v>-8.9999999999999969E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.79</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.81</v>
+      </c>
+      <c r="E4" s="1">
+        <f>SUM(-C4,D4)</f>
+        <v>2.0000000000000018E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.81</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.86</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" ref="E5:E7" si="1">SUM(-C5,D5)</f>
+        <v>4.9999999999999933E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.49</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.37</v>
+      </c>
+      <c r="E6" s="1">
+        <f>SUM(-C6,D6)</f>
+        <v>-0.12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.69</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="1">
+        <f t="shared" si="1"/>
+        <v>-0.69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>